<commit_message>
add first afternoon session
</commit_message>
<xml_diff>
--- a/data/Rocio_tomato_modified.xlsx
+++ b/data/Rocio_tomato_modified.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorondo/Repos/RworkshopUdS_2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B27D369-2387-944C-BF5D-D41F13251835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD383C3-F60A-1342-B017-08F01D9E634F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="11500" xr2:uid="{90870DF7-A05D-405A-A21B-EDD77005A3B8}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="19420" windowHeight="11500" xr2:uid="{90870DF7-A05D-405A-A21B-EDD77005A3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,6 @@
     <t>rep</t>
   </si>
   <si>
-    <t>chlorotic area</t>
-  </si>
-  <si>
-    <t>total area</t>
-  </si>
-  <si>
     <t>mock</t>
   </si>
   <si>
@@ -66,6 +60,12 @@
   </si>
   <si>
     <t>pathogn</t>
+  </si>
+  <si>
+    <t>total.area</t>
+  </si>
+  <si>
+    <t>chlorotic.area</t>
   </si>
 </sst>
 </file>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49393570-5FA6-4B65-B502-63FB37254930}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" zoomScale="232" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -471,16 +471,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -488,10 +488,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>2663192</v>
@@ -505,10 +505,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>3466704</v>
@@ -522,10 +522,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>3604993</v>
@@ -539,10 +539,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1">
         <v>3605450</v>
@@ -556,10 +556,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1">
         <v>2323251</v>
@@ -573,10 +573,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1">
         <v>2938431</v>
@@ -590,10 +590,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>3565796</v>
@@ -607,10 +607,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>3036358</v>
@@ -624,10 +624,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>3145316</v>
@@ -641,10 +641,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>3113820</v>
@@ -658,10 +658,10 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>3296435</v>
@@ -675,10 +675,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>2900551</v>
@@ -692,10 +692,10 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14">
         <v>3086323</v>
@@ -709,10 +709,10 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>2932714</v>
@@ -726,10 +726,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D16">
         <v>4389281</v>
@@ -743,10 +743,10 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>2551986</v>
@@ -760,10 +760,10 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>3199088</v>
@@ -777,10 +777,10 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D19">
         <v>2827940</v>
@@ -794,10 +794,10 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>2383642</v>
@@ -811,10 +811,10 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D21">
         <v>2922258</v>
@@ -828,10 +828,10 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D22">
         <v>2885750</v>
@@ -845,10 +845,10 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D23">
         <v>2533136</v>
@@ -862,10 +862,10 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D24">
         <v>2807570</v>
@@ -879,10 +879,10 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D25">
         <v>2656129</v>
@@ -896,10 +896,10 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D26">
         <v>4256154</v>
@@ -913,10 +913,10 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D27">
         <v>2480123</v>
@@ -930,10 +930,10 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D28">
         <v>2988388</v>
@@ -947,10 +947,10 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D29">
         <v>3678952</v>
@@ -964,10 +964,10 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D30">
         <v>2401455</v>
@@ -981,10 +981,10 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D31">
         <v>3405497</v>
@@ -998,10 +998,10 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D32">
         <v>3509487</v>
@@ -1015,10 +1015,10 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D33">
         <v>2217579</v>
@@ -1032,10 +1032,10 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D34">
         <v>2416968</v>
@@ -1049,10 +1049,10 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D35">
         <v>3506350</v>
@@ -1066,10 +1066,10 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D36">
         <v>3289677</v>
@@ -1083,10 +1083,10 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D37">
         <v>3324250</v>
@@ -1100,10 +1100,10 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D38">
         <v>1912381</v>
@@ -1117,10 +1117,10 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D39">
         <v>1490263</v>
@@ -1134,10 +1134,10 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D40">
         <v>1329052</v>
@@ -1151,10 +1151,10 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D41">
         <v>1388155</v>
@@ -1168,10 +1168,10 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D42">
         <v>2124967</v>
@@ -1185,10 +1185,10 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D43">
         <v>1186987</v>
@@ -1202,10 +1202,10 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D44">
         <v>1259995</v>
@@ -1219,10 +1219,10 @@
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D45">
         <v>1034441</v>
@@ -1236,10 +1236,10 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D46">
         <v>1177668</v>
@@ -1253,10 +1253,10 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D47">
         <v>1503442</v>
@@ -1270,10 +1270,10 @@
         <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D48">
         <v>1063699</v>
@@ -1287,10 +1287,10 @@
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D49">
         <v>1258514</v>

</xml_diff>